<commit_message>
Add doc for fix bug.
</commit_message>
<xml_diff>
--- a/RiskEval test/Test/New/20160709/RiskEval_Test_Script.xlsx
+++ b/RiskEval test/Test/New/20160709/RiskEval_Test_Script.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="4530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="4530" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ภาพรวม" sheetId="1" r:id="rId1"/>
@@ -310,7 +310,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="143">
   <si>
     <t>ทดสอบการลงทะเบียน (ส่วนราชการ รัฐวิสาหกิจ หน่วยงานอื่นของรัฐ จังหวัด และกลุ่มจังหวัด)</t>
   </si>
@@ -391,9 +391,6 @@
   </si>
   <si>
     <t>การทำแบบประเมิณจะต้องทำเรียงลำดับจากข้อแรกไปยังข้อสุดท้าย จะไม่สามารถทำข้ามข้อได้</t>
-  </si>
-  <si>
-    <t>ทดสอบการแสดงข้อมูลโครงการ</t>
   </si>
   <si>
     <t>ค้นหาโครงการที่ผ่านการพิจารณาจากรัฐสภา</t>
@@ -1025,19 +1022,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1062,21 +1051,29 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1396,64 +1393,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="4" customWidth="1"/>
-    <col min="2" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="18.125" style="4" customWidth="1"/>
+    <col min="2" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1463,9 +1460,6 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1474,52 +1468,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.125" customWidth="1"/>
     <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="G1" s="43"/>
+      <c r="H1" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="27" t="s">
+      <c r="I1" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="J1" s="46"/>
+      <c r="K1" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="48"/>
-      <c r="K1" s="45" t="s">
+      <c r="L1" s="43"/>
+      <c r="M1" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="49" t="s">
+      <c r="N1" s="47"/>
+      <c r="O1" s="28" t="s">
         <v>50</v>
-      </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="28" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="49"/>
       <c r="E2" s="8"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -1534,35 +1528,35 @@
     </row>
     <row r="3" spans="1:15" s="16" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="D3" s="42"/>
+      <c r="E3" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="F3" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="42"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="51" t="s">
+        <v>136</v>
+      </c>
+      <c r="J3" s="52"/>
+      <c r="K3" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="14" t="s">
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="39" t="s">
         <v>54</v>
-      </c>
-      <c r="F3" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="J3" s="43"/>
-      <c r="K3" s="40" t="s">
-        <v>119</v>
-      </c>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="39" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1591,11 +1585,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
@@ -1603,6 +1592,11 @@
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1618,58 +1612,58 @@
   <dimension ref="A1:P231"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6:N6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.875" customWidth="1"/>
+    <col min="9" max="9" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="G1" s="43"/>
+      <c r="H1" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="27" t="s">
+      <c r="I1" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="J1" s="46"/>
+      <c r="K1" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="48"/>
-      <c r="K1" s="45" t="s">
+      <c r="L1" s="43"/>
+      <c r="M1" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="49" t="s">
+      <c r="N1" s="47"/>
+      <c r="O1" s="28" t="s">
         <v>50</v>
-      </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="28" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="49"/>
       <c r="E2" s="8"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -1684,396 +1678,396 @@
     </row>
     <row r="3" spans="1:16" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="42"/>
+      <c r="E3" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="F3" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="14" t="s">
+      <c r="G3" s="42"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="19" t="s">
         <v>54</v>
-      </c>
-      <c r="F3" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="40" t="s">
-        <v>123</v>
-      </c>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="19" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:16" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="41"/>
+        <v>69</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="42"/>
       <c r="E4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="42"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="19" t="s">
         <v>54</v>
-      </c>
-      <c r="F4" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="40" t="s">
-        <v>123</v>
-      </c>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="19" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="41"/>
+        <v>77</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="42"/>
       <c r="E5" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="42"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="19" t="s">
         <v>54</v>
-      </c>
-      <c r="F5" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="41"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="40" t="s">
-        <v>123</v>
-      </c>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="19" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="41"/>
+        <v>84</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="42"/>
       <c r="E6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="42"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="L6" s="57"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="19" t="s">
         <v>54</v>
-      </c>
-      <c r="F6" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="41"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="54" t="s">
-        <v>123</v>
-      </c>
-      <c r="L6" s="54"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="19" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="41"/>
+        <v>85</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="42"/>
       <c r="E7" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="41"/>
+        <v>53</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="42"/>
       <c r="H7" s="12"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
       <c r="O7" s="19"/>
       <c r="P7" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="41"/>
+        <v>86</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="42"/>
       <c r="E8" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="41"/>
+        <v>53</v>
+      </c>
+      <c r="F8" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="42"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
       <c r="O8" s="19"/>
       <c r="P8" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="41"/>
+        <v>87</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="42"/>
       <c r="E9" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="41"/>
+        <v>53</v>
+      </c>
+      <c r="F9" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="42"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
       <c r="O9" s="19"/>
       <c r="P9" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="41"/>
+      <c r="C10" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="42"/>
       <c r="E10" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="41"/>
+        <v>53</v>
+      </c>
+      <c r="F10" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="42"/>
       <c r="H10" s="12"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
       <c r="O10" s="19"/>
       <c r="P10" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="41"/>
+        <v>121</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="42"/>
       <c r="E11" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="41"/>
+        <v>53</v>
+      </c>
+      <c r="F11" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="42"/>
       <c r="H11" s="12"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
-      <c r="N11" s="41"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42"/>
       <c r="O11" s="19"/>
       <c r="P11" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="41"/>
+      <c r="C12" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="42"/>
       <c r="E12" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="41"/>
+        <v>53</v>
+      </c>
+      <c r="F12" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="42"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="42"/>
       <c r="O12" s="19"/>
       <c r="P12" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C13" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="41"/>
+      <c r="C13" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="42"/>
       <c r="E13" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="41"/>
+        <v>53</v>
+      </c>
+      <c r="F13" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="42"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="42"/>
       <c r="O13" s="19"/>
       <c r="P13" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="C14" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="41"/>
+      <c r="C14" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="42"/>
       <c r="E14" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="41"/>
+        <v>53</v>
+      </c>
+      <c r="F14" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="42"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="42"/>
       <c r="O14" s="19"/>
       <c r="P14" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="C15" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="41"/>
+      <c r="C15" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="42"/>
       <c r="E15" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="41"/>
+        <v>53</v>
+      </c>
+      <c r="F15" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="42"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="40"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="41"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="42"/>
+      <c r="N15" s="42"/>
       <c r="O15" s="19"/>
       <c r="P15" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
@@ -2139,7 +2133,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C41" s="3"/>
-      <c r="I41" s="56"/>
+      <c r="I41" s="41"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" s="3"/>
@@ -2695,61 +2689,228 @@
     </row>
   </sheetData>
   <mergeCells count="72">
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="M14:N14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.125" style="4" customWidth="1"/>
+    <col min="2" max="14" width="8.875" style="4"/>
+    <col min="15" max="15" width="16.875" style="4" customWidth="1"/>
+    <col min="16" max="16384" width="8.875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="44"/>
+      <c r="E1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="43"/>
+      <c r="H1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="46"/>
+      <c r="K1" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="43"/>
+      <c r="M1" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="47"/>
+      <c r="O1" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+    </row>
+    <row r="3" spans="1:15" s="16" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="42"/>
+      <c r="E3" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="42"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="51" t="s">
+        <v>137</v>
+      </c>
+      <c r="J3" s="52"/>
+      <c r="K3" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="16" customFormat="1" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="42"/>
+      <c r="E4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="42"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="J4" s="52"/>
+      <c r="K4" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" s="42"/>
+      <c r="M4" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="N4" s="53"/>
+      <c r="O4" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="I4:J4"/>
@@ -2774,64 +2935,61 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="4" customWidth="1"/>
-    <col min="2" max="14" width="8.85546875" style="4"/>
-    <col min="15" max="15" width="16.85546875" style="4" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="17.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:15" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="G1" s="43"/>
+      <c r="H1" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="J1" s="46"/>
+      <c r="K1" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="48"/>
-      <c r="K1" s="45" t="s">
+      <c r="L1" s="43"/>
+      <c r="M1" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="49" t="s">
+      <c r="N1" s="47"/>
+      <c r="O1" s="21" t="s">
         <v>50</v>
-      </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="18" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="49"/>
       <c r="E2" s="8"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -2846,74 +3004,241 @@
     </row>
     <row r="3" spans="1:15" s="16" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="42"/>
+      <c r="E3" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="42"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="42" t="s">
-        <v>138</v>
-      </c>
-      <c r="J3" s="43"/>
-      <c r="K3" s="40" t="s">
+    </row>
+    <row r="4" spans="1:15" s="16" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="16" customFormat="1" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="41"/>
+      <c r="C4" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="42"/>
       <c r="E4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="42"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="42" t="s">
-        <v>139</v>
-      </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="L4" s="41"/>
-      <c r="M4" s="44" t="s">
+    </row>
+    <row r="5" spans="1:15" s="16" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="N4" s="44"/>
-      <c r="O4" s="23" t="s">
-        <v>72</v>
-      </c>
+      <c r="B5" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="42"/>
+      <c r="E5" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="42"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="16" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="42"/>
+      <c r="E6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="42"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="16" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="42"/>
+      <c r="E7" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="42"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
+      <c r="O7" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="16" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="42"/>
+      <c r="E8" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="42"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="16" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="42"/>
+      <c r="E9" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="42"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
+      <c r="O9" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="3"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="3"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="3"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="3"/>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C46" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="42">
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
@@ -2926,6 +3251,233 @@
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.875" customWidth="1"/>
+    <col min="10" max="10" width="15.125" customWidth="1"/>
+    <col min="15" max="15" width="17.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="44"/>
+      <c r="E1" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="43"/>
+      <c r="H1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="46"/>
+      <c r="K1" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="43"/>
+      <c r="M1" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="47"/>
+      <c r="O1" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+    </row>
+    <row r="3" spans="1:15" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="42"/>
+      <c r="E3" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="42"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" s="52"/>
+      <c r="K3" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="16" customFormat="1" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="42"/>
+      <c r="E4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" s="42"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="J4" s="52"/>
+      <c r="K4" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="16" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="42"/>
+      <c r="E5" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="51" t="s">
+        <v>91</v>
+      </c>
+      <c r="G5" s="52"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="J5" s="52"/>
+      <c r="K5" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="52"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="55"/>
+      <c r="O5" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="I4:J4"/>
@@ -2938,61 +3490,61 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="G1" s="43"/>
+      <c r="H1" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="20" t="s">
+      <c r="I1" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="J1" s="46"/>
+      <c r="K1" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="48"/>
-      <c r="K1" s="45" t="s">
+      <c r="L1" s="43"/>
+      <c r="M1" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="49" t="s">
+      <c r="N1" s="47"/>
+      <c r="O1" s="25" t="s">
         <v>50</v>
-      </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="21" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="49"/>
       <c r="E2" s="8"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -3005,225 +3557,114 @@
       <c r="N2" s="11"/>
       <c r="O2" s="11"/>
     </row>
-    <row r="3" spans="1:15" s="16" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="42"/>
+      <c r="E3" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="42"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="J3" s="52"/>
+      <c r="K3" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="16" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="41"/>
+        <v>95</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="42"/>
       <c r="E4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="42"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="J4" s="52"/>
+      <c r="K4" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="40" t="s">
+    </row>
+    <row r="5" spans="1:15" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="16" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="41"/>
+      <c r="C5" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="42"/>
       <c r="E5" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="42"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" s="52"/>
+      <c r="K5" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="G5" s="41"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" s="16" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="40" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="41"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="16" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="G7" s="41"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="16" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="41"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" s="16" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="G9" s="41"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="19" t="s">
-        <v>55</v>
-      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="26"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="3"/>
+      <c r="C11" s="5"/>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="3"/>
@@ -3231,47 +3672,18 @@
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" s="3"/>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C32" s="3"/>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C39" s="3"/>
-    </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C46" s="3"/>
-    </row>
   </sheetData>
-  <mergeCells count="42">
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="M7:N7"/>
+  <mergeCells count="22">
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
@@ -3291,63 +3703,62 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.125" customWidth="1"/>
+    <col min="10" max="10" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="G1" s="43"/>
+      <c r="H1" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="20" t="s">
+      <c r="I1" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="J1" s="46"/>
+      <c r="K1" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="48"/>
-      <c r="K1" s="45" t="s">
+      <c r="L1" s="43"/>
+      <c r="M1" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="49" t="s">
+      <c r="N1" s="47"/>
+      <c r="O1" s="25" t="s">
         <v>50</v>
-      </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="21" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="49"/>
       <c r="E2" s="8"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -3360,107 +3771,104 @@
       <c r="N2" s="11"/>
       <c r="O2" s="11"/>
     </row>
-    <row r="3" spans="1:15" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="16" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="42"/>
+      <c r="E3" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="42"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="51" t="s">
+        <v>131</v>
+      </c>
+      <c r="J3" s="52"/>
+      <c r="K3" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="J3" s="43"/>
-      <c r="K3" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="16" customFormat="1" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="41"/>
+        <v>69</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="42"/>
       <c r="E4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="42"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="51" t="s">
+        <v>132</v>
+      </c>
+      <c r="J4" s="52"/>
+      <c r="K4" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="16" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:15" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="41"/>
+        <v>77</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="42"/>
       <c r="E5" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" s="42"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="J5" s="52"/>
+      <c r="K5" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="G5" s="43"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="J5" s="43"/>
-      <c r="K5" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="L5" s="43"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -3493,417 +3901,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" s="48"/>
-      <c r="K1" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-    </row>
-    <row r="3" spans="1:15" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="J3" s="43"/>
-      <c r="K3" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="42" t="s">
-        <v>101</v>
-      </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="G5" s="41"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="J5" s="43"/>
-      <c r="K5" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="5"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="3"/>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="10" max="10" width="23" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" s="48"/>
-      <c r="K1" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-    </row>
-    <row r="3" spans="1:15" s="16" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="J3" s="43"/>
-      <c r="K3" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="16" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="G5" s="41"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="J5" s="43"/>
-      <c r="K5" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O18"/>
@@ -3914,86 +3911,86 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="24" t="s">
+      <c r="F1" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="G1" s="43"/>
+      <c r="H1" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="24" t="s">
+      <c r="I1" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="J1" s="46"/>
+      <c r="K1" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="48"/>
-      <c r="K1" s="45" t="s">
+      <c r="L1" s="43"/>
+      <c r="M1" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="49" t="s">
+      <c r="N1" s="47"/>
+      <c r="O1" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="25" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="2" spans="1:15" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="27" t="s">
+      <c r="F2" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="G2" s="43"/>
+      <c r="H2" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="27" t="s">
+      <c r="I2" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="47" t="s">
+      <c r="J2" s="46"/>
+      <c r="K2" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="48"/>
-      <c r="K2" s="45" t="s">
+      <c r="L2" s="43"/>
+      <c r="M2" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="45"/>
-      <c r="M2" s="49" t="s">
+      <c r="N2" s="47"/>
+      <c r="O2" s="28" t="s">
         <v>50</v>
-      </c>
-      <c r="N2" s="49"/>
-      <c r="O2" s="28" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" s="7"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="51"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="49"/>
       <c r="E3" s="8"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
@@ -4008,68 +4005,68 @@
     </row>
     <row r="4" spans="1:15" s="16" customFormat="1" ht="98.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="42"/>
+      <c r="E4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="14" t="s">
+      <c r="G4" s="42"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="J4" s="52"/>
+      <c r="K4" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="19" t="s">
         <v>54</v>
-      </c>
-      <c r="F4" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="19" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="16" customFormat="1" ht="98.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="41"/>
+      <c r="D5" s="42"/>
       <c r="E5" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="42"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="J5" s="52"/>
+      <c r="K5" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="19" t="s">
         <v>54</v>
-      </c>
-      <c r="F5" s="40" t="s">
-        <v>110</v>
-      </c>
-      <c r="G5" s="41"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="J5" s="43"/>
-      <c r="K5" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="19" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -4089,6 +4086,16 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M4:N4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="M1:N1"/>
@@ -4102,16 +4109,6 @@
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4121,59 +4118,59 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="G1" s="43"/>
+      <c r="H1" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="27" t="s">
+      <c r="I1" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="J1" s="46"/>
+      <c r="K1" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="48"/>
-      <c r="K1" s="45" t="s">
+      <c r="L1" s="43"/>
+      <c r="M1" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="49" t="s">
+      <c r="N1" s="47"/>
+      <c r="O1" s="28" t="s">
         <v>50</v>
-      </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="28" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="49"/>
       <c r="E2" s="8"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -4188,68 +4185,68 @@
     </row>
     <row r="3" spans="1:15" s="16" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="42"/>
+      <c r="E3" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="14" t="s">
+      <c r="G3" s="42"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="J3" s="52"/>
+      <c r="K3" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="19" t="s">
         <v>54</v>
-      </c>
-      <c r="F3" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="J3" s="43"/>
-      <c r="K3" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="23" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:15" s="16" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="41"/>
+        <v>69</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="42"/>
       <c r="E4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="42"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="J4" s="52"/>
+      <c r="K4" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="19" t="s">
         <v>54</v>
-      </c>
-      <c r="F4" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="40" t="s">
-        <v>116</v>
-      </c>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="19" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -4267,8 +4264,19 @@
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C16" s="3"/>
     </row>
+    <row r="25" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M3:N3"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
@@ -4278,14 +4286,6 @@
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4295,60 +4295,63 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P72"/>
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:P71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:N3"/>
+      <selection activeCell="F4" sqref="F4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.25" customWidth="1"/>
     <col min="16" max="16" width="47" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="29" t="s">
+      <c r="F1" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="G1" s="43"/>
+      <c r="H1" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="29" t="s">
+      <c r="I1" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="J1" s="46"/>
+      <c r="K1" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="48"/>
-      <c r="K1" s="45" t="s">
+      <c r="L1" s="43"/>
+      <c r="M1" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="49" t="s">
+      <c r="N1" s="47"/>
+      <c r="O1" s="30" t="s">
         <v>50</v>
-      </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="30" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="49"/>
       <c r="E2" s="8"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -4363,114 +4366,89 @@
     </row>
     <row r="3" spans="1:16" s="16" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="42"/>
+      <c r="E3" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="41"/>
+      <c r="G3" s="42"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="40" t="s">
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="41"/>
-      <c r="M3" s="57" t="s">
-        <v>142</v>
-      </c>
-      <c r="N3" s="57"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="N3" s="56"/>
       <c r="O3" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:16" s="16" customFormat="1" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="42"/>
+      <c r="E4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="50" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="40" t="s">
-        <v>141</v>
-      </c>
-      <c r="G4" s="41"/>
+      <c r="G4" s="42"/>
       <c r="H4" s="12"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
       <c r="O4" s="23"/>
-      <c r="P4" s="55" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" s="16" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="41"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="55" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="P4" s="40" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="26"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C11" s="5"/>
-    </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C59" s="3"/>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C72" s="3"/>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C58" s="3"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="17">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
@@ -4483,16 +4461,6 @@
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>